<commit_message>
Mod by yxq @20171221
</commit_message>
<xml_diff>
--- a/xboost/com.xboost.business/src/main/webapp/static/excelTemplate/Test - Settings - Parameters.xlsx
+++ b/xboost/com.xboost.business/src/main/webapp/static/excelTemplate/Test - Settings - Parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19104" windowHeight="7787"/>
+    <workbookView windowWidth="18528" windowHeight="7787"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25">
   <si>
     <t>ID</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>16:00-17:00</t>
+  </si>
+  <si>
+    <t>时间间隔</t>
   </si>
 </sst>
 </file>
@@ -95,9 +98,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -118,9 +121,114 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -140,114 +248,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -270,6 +273,126 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -300,60 +423,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -361,72 +430,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -479,45 +482,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -529,26 +493,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -576,6 +520,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -584,10 +587,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -596,143 +599,144 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1081,10 +1085,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -1231,6 +1235,20 @@
         <v>23</v>
       </c>
       <c r="D10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="4">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
mod @20171228 by yxq
</commit_message>
<xml_diff>
--- a/xboost/com.xboost.business/src/main/webapp/static/excelTemplate/Test - Settings - Parameters.xlsx
+++ b/xboost/com.xboost.business/src/main/webapp/static/excelTemplate/Test - Settings - Parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19104" windowHeight="7787"/>
+    <workbookView windowWidth="18528" windowHeight="7787"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43">
   <si>
     <t>ID</t>
   </si>
@@ -72,6 +72,9 @@
     <t>集配站集散点人效（p）</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>duration_peak</t>
   </si>
   <si>
@@ -90,6 +93,15 @@
     <t>17:00 - 19:00</t>
   </si>
   <si>
+    <t>price_type</t>
+  </si>
+  <si>
+    <t>时间周期</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
@@ -130,6 +142,9 @@
   </si>
   <si>
     <t>派件串连耗时</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -138,9 +153,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -160,7 +175,128 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -175,133 +311,12 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -312,90 +327,180 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -403,96 +508,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -623,17 +638,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -648,16 +657,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -679,6 +688,45 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -687,39 +735,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -728,10 +743,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -740,137 +755,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -908,6 +923,18 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -928,6 +955,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1280,10 +1310,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1399,17 +1429,17 @@
       <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="9">
-        <v>1</v>
+      <c r="B6" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>6</v>
@@ -1423,13 +1453,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>6</v>
@@ -1440,39 +1470,39 @@
         <v>6</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C8" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D9" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E9" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>13</v>
+      <c r="F9" s="20" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1480,19 +1510,19 @@
         <v>6</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="9">
-        <v>300</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1500,16 +1530,16 @@
         <v>6</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E11" s="9">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>6</v>
@@ -1520,38 +1550,38 @@
         <v>6</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D12" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="9">
+        <v>500</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="D13" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="19" t="s">
+      <c r="E13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="11" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1559,39 +1589,39 @@
       <c r="A14" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="9">
-        <v>3</v>
+      <c r="B14" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="C14" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D15" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E15" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="9">
-        <v>3</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="25" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1603,16 +1633,16 @@
         <v>3</v>
       </c>
       <c r="C16" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="E16" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>13</v>
+      <c r="F16" s="11" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1623,13 +1653,13 @@
         <v>3</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>6</v>
@@ -1643,13 +1673,13 @@
         <v>3</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>13</v>
@@ -1663,13 +1693,13 @@
         <v>3</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="F19" s="11" t="s">
         <v>6</v>
@@ -1683,16 +1713,16 @@
         <v>3</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1703,13 +1733,13 @@
         <v>3</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="9">
-        <v>300</v>
+        <v>38</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>6</v>
@@ -1723,13 +1753,13 @@
         <v>3</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="9">
-        <v>500</v>
+        <v>41</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="F22" s="11" t="s">
         <v>6</v>
@@ -1743,35 +1773,95 @@
         <v>3</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D23" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="9">
+        <v>300</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="9">
+        <v>3</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="9">
+        <v>500</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="9">
+        <v>3</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="D25" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="18">
+      <c r="E25" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="9">
         <v>3</v>
       </c>
-      <c r="C24" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D24" s="19" t="s">
+      <c r="C26" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="18" t="s">
+      <c r="D26" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="20" t="s">
+      <c r="E26" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" s="25" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>